<commit_message>
Trying to wrap this up
</commit_message>
<xml_diff>
--- a/acc_table.xlsx
+++ b/acc_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,53 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dan\_Remote_projects\ccp-sROS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57B1F010-F1A1-4D3F-8580-635C659F7A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90172537-918E-462F-8DF2-0FAFE73B2642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="acc_table" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Call</t>
   </si>
   <si>
-    <t>Fit.criteria.Min.max.accuracy</t>
-  </si>
-  <si>
-    <t>Fit.criteria.MAE</t>
-  </si>
-  <si>
-    <t>Fit.criteria.MedAE</t>
-  </si>
-  <si>
-    <t>Fit.criteria.MAPE</t>
-  </si>
-  <si>
-    <t>Fit.criteria.MSE</t>
-  </si>
-  <si>
-    <t>Fit.criteria.RMSE</t>
-  </si>
-  <si>
-    <t>Fit.criteria.NRMSE.mean</t>
-  </si>
-  <si>
-    <t>Fit.criteria.NRMSE.median</t>
-  </si>
-  <si>
-    <t>Fit.criteria.Efron.r.squared</t>
-  </si>
-  <si>
-    <t>Fit.criteria.CV.prcnt</t>
-  </si>
-  <si>
     <t>lm(formula = ROS ~ I(isi.m^2) - 1, data = s.fires.con)</t>
   </si>
   <si>
@@ -80,12 +67,90 @@
   </si>
   <si>
     <t xml:space="preserve">nls(formula = ROS ~ 25 * (1 - exp(-b * ISI))^c, data = s.fires.mod %&gt;% </t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Conifer (excluding PPDF)</t>
+  </si>
+  <si>
+    <t>All fires, PPDF90C</t>
+  </si>
+  <si>
+    <t>Ones I want:</t>
+  </si>
+  <si>
+    <t>sf.crisimCon.mod</t>
+  </si>
+  <si>
+    <t>Con</t>
+  </si>
+  <si>
+    <t>Predictors</t>
+  </si>
+  <si>
+    <t>ISIm</t>
+  </si>
+  <si>
+    <t>ISI</t>
+  </si>
+  <si>
+    <t>ISIm, SFC</t>
+  </si>
+  <si>
+    <t>ISI, SFC</t>
+  </si>
+  <si>
+    <t>sf.crisiCon.mod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nls(formula = ROS ~ 25 * (1 - exp(-b * isi.m))^c, data = s.fires.mod %&gt;% </t>
+  </si>
+  <si>
+    <t>con.lm.mod</t>
+  </si>
+  <si>
+    <t>sros.ISI2.mod</t>
+  </si>
+  <si>
+    <t>sros.ISI2SFC.mod</t>
+  </si>
+  <si>
+    <t>sros.isim2.mod</t>
+  </si>
+  <si>
+    <t>sros.isim2SFC.mod</t>
+  </si>
+  <si>
+    <t>sf.crisi.mod</t>
+  </si>
+  <si>
+    <t>sf.crisim.mod</t>
+  </si>
+  <si>
+    <t>sf.axb.isi.mod</t>
+  </si>
+  <si>
+    <t>nobs</t>
+  </si>
+  <si>
+    <t>Efron R2</t>
+  </si>
+  <si>
+    <t>AIC</t>
+  </si>
+  <si>
+    <t>ISI/ISI.sa5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -621,6 +686,163 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="acc_table"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>isim2.con</v>
+          </cell>
+          <cell r="C2">
+            <v>56</v>
+          </cell>
+          <cell r="D2">
+            <v>0.774896281836155</v>
+          </cell>
+          <cell r="E2">
+            <v>199.798864765536</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>ISI2.agg</v>
+          </cell>
+          <cell r="C3">
+            <v>90</v>
+          </cell>
+          <cell r="D3">
+            <v>0.695859490464528</v>
+          </cell>
+          <cell r="E3">
+            <v>351.72399634026101</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>ISI2SFC.agg</v>
+          </cell>
+          <cell r="C4">
+            <v>82</v>
+          </cell>
+          <cell r="D4">
+            <v>0.75620344033680598</v>
+          </cell>
+          <cell r="E4">
+            <v>306.18379831355401</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>isim2.agg</v>
+          </cell>
+          <cell r="C5">
+            <v>90</v>
+          </cell>
+          <cell r="D5">
+            <v>0.76312115633353605</v>
+          </cell>
+          <cell r="E5">
+            <v>329.22930681027799</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>isim2SFC.agg</v>
+          </cell>
+          <cell r="C6">
+            <v>82</v>
+          </cell>
+          <cell r="D6">
+            <v>0.80728637787344004</v>
+          </cell>
+          <cell r="E6">
+            <v>286.90323328026898</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>crisi.agg</v>
+          </cell>
+          <cell r="C7">
+            <v>90</v>
+          </cell>
+          <cell r="D7">
+            <v>0.74207775828477995</v>
+          </cell>
+          <cell r="E7">
+            <v>338.88914817787901</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>crisim.agg</v>
+          </cell>
+          <cell r="C8">
+            <v>90</v>
+          </cell>
+          <cell r="D8">
+            <v>0.77352340243057605</v>
+          </cell>
+          <cell r="E8">
+            <v>327.18766019001299</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>axb.isi.agg</v>
+          </cell>
+          <cell r="C9">
+            <v>90</v>
+          </cell>
+          <cell r="D9">
+            <v>0.74143205177162796</v>
+          </cell>
+          <cell r="E9">
+            <v>339.11418097653302</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>crisi.con</v>
+          </cell>
+          <cell r="C10">
+            <v>50</v>
+          </cell>
+          <cell r="D10">
+            <v>0.87493746232692504</v>
+          </cell>
+          <cell r="E10">
+            <v>143.57829228489899</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>crisim.con</v>
+          </cell>
+          <cell r="C11">
+            <v>50</v>
+          </cell>
+          <cell r="D11">
+            <v>0.85825277441075398</v>
+          </cell>
+          <cell r="E11">
+            <v>149.83986509868799</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -939,49 +1161,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="59.77734375" customWidth="1"/>
+    <col min="2" max="4" width="22.5546875" customWidth="1"/>
+    <col min="5" max="5" width="68.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="15" max="15" width="11.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1">
         <v>10</v>
+      </c>
+      <c r="L1">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -989,37 +1219,32 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>0.52100000000000002</v>
-      </c>
-      <c r="D2">
-        <v>1.26</v>
-      </c>
-      <c r="E2">
-        <v>0.80400000000000005</v>
-      </c>
-      <c r="F2">
-        <v>0.63100000000000001</v>
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="str">
+        <f>[1]acc_table!B2</f>
+        <v>isim2.con</v>
       </c>
       <c r="G2">
-        <v>3.36</v>
+        <f>[1]acc_table!C2</f>
+        <v>56</v>
       </c>
       <c r="H2">
-        <v>1.83</v>
+        <f>[1]acc_table!D2</f>
+        <v>0.774896281836155</v>
       </c>
       <c r="I2">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="J2">
-        <v>1.24</v>
-      </c>
-      <c r="K2">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="L2">
-        <v>90.6</v>
+        <f>[1]acc_table!E2</f>
+        <v>199.798864765536</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -1027,37 +1252,32 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="D3">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E3">
-        <v>0.64300000000000002</v>
-      </c>
-      <c r="F3">
-        <v>0.56100000000000005</v>
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="str">
+        <f>[1]acc_table!B3</f>
+        <v>ISI2.agg</v>
       </c>
       <c r="G3">
-        <v>2.94</v>
+        <f>[1]acc_table!C3</f>
+        <v>90</v>
       </c>
       <c r="H3">
-        <v>1.71</v>
+        <f>[1]acc_table!D3</f>
+        <v>0.695859490464528</v>
       </c>
       <c r="I3">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="J3">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="K3">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="L3">
-        <v>78.2</v>
+        <f>[1]acc_table!E3</f>
+        <v>351.72399634026101</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1065,37 +1285,32 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="C4">
-        <v>0.65600000000000003</v>
-      </c>
-      <c r="D4">
-        <v>1.03</v>
-      </c>
-      <c r="E4">
-        <v>0.60699999999999998</v>
-      </c>
-      <c r="F4">
-        <v>0.61</v>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="str">
+        <f>[1]acc_table!B4</f>
+        <v>ISI2SFC.agg</v>
       </c>
       <c r="G4">
-        <v>2.41</v>
+        <f>[1]acc_table!C4</f>
+        <v>82</v>
       </c>
       <c r="H4">
-        <v>1.55</v>
+        <f>[1]acc_table!D4</f>
+        <v>0.75620344033680598</v>
       </c>
       <c r="I4">
-        <v>0.70899999999999996</v>
-      </c>
-      <c r="J4">
-        <v>1.04</v>
-      </c>
-      <c r="K4">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="L4">
-        <v>70.900000000000006</v>
+        <f>[1]acc_table!E4</f>
+        <v>306.18379831355401</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1103,37 +1318,32 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="D5">
-        <v>1.05</v>
-      </c>
-      <c r="E5">
-        <v>0.71899999999999997</v>
-      </c>
-      <c r="F5">
-        <v>0.55900000000000005</v>
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="str">
+        <f>[1]acc_table!B5</f>
+        <v>isim2.agg</v>
       </c>
       <c r="G5">
-        <v>2.21</v>
+        <f>[1]acc_table!C5</f>
+        <v>90</v>
       </c>
       <c r="H5">
-        <v>1.49</v>
+        <f>[1]acc_table!D5</f>
+        <v>0.76312115633353605</v>
       </c>
       <c r="I5">
-        <v>0.67900000000000005</v>
-      </c>
-      <c r="J5">
-        <v>0.99199999999999999</v>
-      </c>
-      <c r="K5">
-        <v>0.53600000000000003</v>
-      </c>
-      <c r="L5">
-        <v>67.900000000000006</v>
+        <f>[1]acc_table!E5</f>
+        <v>329.22930681027799</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1141,37 +1351,32 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="D6">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="E6">
-        <v>0.622</v>
-      </c>
-      <c r="F6">
-        <v>0.54700000000000004</v>
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="str">
+        <f>[1]acc_table!B6</f>
+        <v>isim2SFC.agg</v>
       </c>
       <c r="G6">
-        <v>1.84</v>
+        <f>[1]acc_table!C6</f>
+        <v>82</v>
       </c>
       <c r="H6">
-        <v>1.36</v>
+        <f>[1]acc_table!D6</f>
+        <v>0.80728637787344004</v>
       </c>
       <c r="I6">
-        <v>0.61899999999999999</v>
-      </c>
-      <c r="J6">
-        <v>0.90400000000000003</v>
-      </c>
-      <c r="K6">
-        <v>0.63100000000000001</v>
-      </c>
-      <c r="L6">
-        <v>61.9</v>
+        <f>[1]acc_table!E6</f>
+        <v>286.90323328026898</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -1179,37 +1384,32 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="D7">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E7">
-        <v>0.80700000000000005</v>
-      </c>
-      <c r="F7">
-        <v>0.7</v>
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="str">
+        <f>[1]acc_table!B7</f>
+        <v>crisi.agg</v>
       </c>
       <c r="G7">
-        <v>2.4500000000000002</v>
+        <f>[1]acc_table!C7</f>
+        <v>90</v>
       </c>
       <c r="H7">
-        <v>1.56</v>
+        <f>[1]acc_table!D7</f>
+        <v>0.74207775828477995</v>
       </c>
       <c r="I7">
-        <v>0.71399999999999997</v>
-      </c>
-      <c r="J7">
-        <v>1.04</v>
-      </c>
-      <c r="K7">
-        <v>0.48699999999999999</v>
-      </c>
-      <c r="L7">
-        <v>71.400000000000006</v>
+        <f>[1]acc_table!E7</f>
+        <v>338.88914817787901</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -1217,37 +1417,32 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="D8">
-        <v>1.05</v>
-      </c>
-      <c r="E8">
-        <v>0.85099999999999998</v>
-      </c>
-      <c r="F8">
-        <v>0.65</v>
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="str">
+        <f>[1]acc_table!B8</f>
+        <v>crisim.agg</v>
       </c>
       <c r="G8">
-        <v>2.1800000000000002</v>
+        <f>[1]acc_table!C8</f>
+        <v>90</v>
       </c>
       <c r="H8">
-        <v>1.48</v>
+        <f>[1]acc_table!D8</f>
+        <v>0.77352340243057605</v>
       </c>
       <c r="I8">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="J8">
-        <v>0.98499999999999999</v>
-      </c>
-      <c r="K8">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="L8">
-        <v>69.2</v>
+        <f>[1]acc_table!E8</f>
+        <v>327.18766019001299</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -1255,37 +1450,32 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>0.61</v>
-      </c>
-      <c r="D9">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E9">
-        <v>0.81799999999999995</v>
-      </c>
-      <c r="F9">
-        <v>0.71599999999999997</v>
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="str">
+        <f>[1]acc_table!B9</f>
+        <v>axb.isi.agg</v>
       </c>
       <c r="G9">
-        <v>2.46</v>
+        <f>[1]acc_table!C9</f>
+        <v>90</v>
       </c>
       <c r="H9">
-        <v>1.57</v>
+        <f>[1]acc_table!D9</f>
+        <v>0.74143205177162796</v>
       </c>
       <c r="I9">
-        <v>0.71599999999999997</v>
-      </c>
-      <c r="J9">
-        <v>1.05</v>
-      </c>
-      <c r="K9">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="L9">
-        <v>71.599999999999994</v>
+        <f>[1]acc_table!E9</f>
+        <v>339.11418097653302</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -1293,37 +1483,86 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="D10">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="E10">
-        <v>0.54</v>
-      </c>
-      <c r="F10">
-        <v>0.59899999999999998</v>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="str">
+        <f>[1]acc_table!B10</f>
+        <v>crisi.con</v>
       </c>
       <c r="G10">
-        <v>0.96099999999999997</v>
+        <f>[1]acc_table!C10</f>
+        <v>50</v>
       </c>
       <c r="H10">
-        <v>0.98</v>
+        <f>[1]acc_table!D10</f>
+        <v>0.87493746232692504</v>
       </c>
       <c r="I10">
-        <v>0.52100000000000002</v>
-      </c>
-      <c r="J10">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="K10">
-        <v>0.78100000000000003</v>
-      </c>
-      <c r="L10">
-        <v>52.1</v>
+        <f>[1]acc_table!E10</f>
+        <v>143.57829228489899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="str">
+        <f>[1]acc_table!B11</f>
+        <v>crisim.con</v>
+      </c>
+      <c r="G11">
+        <f>[1]acc_table!C11</f>
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <f>[1]acc_table!D11</f>
+        <v>0.85825277441075398</v>
+      </c>
+      <c r="I11">
+        <f>[1]acc_table!E11</f>
+        <v>149.83986509868799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1334,6 +1573,20 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" zoomScale="122" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{219619fd-75dc-48cb-820d-8f683a95dd8b}" enabled="1" method="Privileged" siteId="{05c95b33-90ca-49d5-b644-288b930b912b}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
Commit commit commit commit commit
</commit_message>
<xml_diff>
--- a/acc_table.xlsx
+++ b/acc_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dan\_Remote_projects\ccp-sROS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90172537-918E-462F-8DF2-0FAFE73B2642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E7DDFB-3B82-4A58-80DA-0EE429C8C356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Call</t>
   </si>
@@ -145,12 +145,24 @@
   </si>
   <si>
     <t>ISI/ISI.sa5</t>
+  </si>
+  <si>
+    <t>Mean.agg</t>
+  </si>
+  <si>
+    <t>Mean.con</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -287,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,8 +479,32 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7ABDD8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB5E6A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8181"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -583,6 +619,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -628,8 +673,26 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="16" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -677,6 +740,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF8181"/>
+      <color rgb="FFB5E6A2"/>
+      <color rgb="FF7ABDD8"/>
+      <color rgb="FFFFA74F"/>
+      <color rgb="FFCC6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -707,10 +779,19 @@
             <v>56</v>
           </cell>
           <cell r="D2">
-            <v>0.774896281836155</v>
+            <v>199.8</v>
           </cell>
           <cell r="E2">
-            <v>199.798864765536</v>
+            <v>0.77500000000000002</v>
+          </cell>
+          <cell r="F2">
+            <v>0.57999999999999996</v>
+          </cell>
+          <cell r="G2">
+            <v>2.34</v>
+          </cell>
+          <cell r="H2">
+            <v>5.26</v>
           </cell>
         </row>
         <row r="3">
@@ -721,10 +802,19 @@
             <v>90</v>
           </cell>
           <cell r="D3">
-            <v>0.695859490464528</v>
+            <v>351.7</v>
           </cell>
           <cell r="E3">
-            <v>351.72399634026101</v>
+            <v>0.69599999999999995</v>
+          </cell>
+          <cell r="F3">
+            <v>0.4</v>
+          </cell>
+          <cell r="G3">
+            <v>1.6</v>
+          </cell>
+          <cell r="H3">
+            <v>3.59</v>
           </cell>
         </row>
         <row r="4">
@@ -735,10 +825,19 @@
             <v>82</v>
           </cell>
           <cell r="D4">
-            <v>0.75620344033680598</v>
+            <v>306.2</v>
           </cell>
           <cell r="E4">
-            <v>306.18379831355401</v>
+            <v>0.75600000000000001</v>
+          </cell>
+          <cell r="F4">
+            <v>1.1599999999999999</v>
+          </cell>
+          <cell r="G4">
+            <v>2.21</v>
+          </cell>
+          <cell r="H4">
+            <v>3.97</v>
           </cell>
         </row>
         <row r="5">
@@ -749,10 +848,19 @@
             <v>90</v>
           </cell>
           <cell r="D5">
-            <v>0.76312115633353605</v>
+            <v>329.2</v>
           </cell>
           <cell r="E5">
-            <v>329.22930681027799</v>
+            <v>0.76300000000000001</v>
+          </cell>
+          <cell r="F5">
+            <v>0.42</v>
+          </cell>
+          <cell r="G5">
+            <v>1.67</v>
+          </cell>
+          <cell r="H5">
+            <v>3.76</v>
           </cell>
         </row>
         <row r="6">
@@ -763,10 +871,19 @@
             <v>82</v>
           </cell>
           <cell r="D6">
-            <v>0.80728637787344004</v>
+            <v>286.89999999999998</v>
           </cell>
           <cell r="E6">
-            <v>286.90323328026898</v>
+            <v>0.80700000000000005</v>
+          </cell>
+          <cell r="F6">
+            <v>0.9</v>
+          </cell>
+          <cell r="G6">
+            <v>2.0499999999999998</v>
+          </cell>
+          <cell r="H6">
+            <v>3.97</v>
           </cell>
         </row>
         <row r="7">
@@ -777,10 +894,19 @@
             <v>90</v>
           </cell>
           <cell r="D7">
-            <v>0.74207775828477995</v>
+            <v>338.9</v>
           </cell>
           <cell r="E7">
-            <v>338.88914817787901</v>
+            <v>0.74199999999999999</v>
+          </cell>
+          <cell r="F7">
+            <v>0.68</v>
+          </cell>
+          <cell r="G7">
+            <v>2.2400000000000002</v>
+          </cell>
+          <cell r="H7">
+            <v>4.22</v>
           </cell>
         </row>
         <row r="8">
@@ -791,10 +917,19 @@
             <v>90</v>
           </cell>
           <cell r="D8">
-            <v>0.77352340243057605</v>
+            <v>327.2</v>
           </cell>
           <cell r="E8">
-            <v>327.18766019001299</v>
+            <v>0.77400000000000002</v>
+          </cell>
+          <cell r="F8">
+            <v>0.65</v>
+          </cell>
+          <cell r="G8">
+            <v>2.17</v>
+          </cell>
+          <cell r="H8">
+            <v>4.1399999999999997</v>
           </cell>
         </row>
         <row r="9">
@@ -805,10 +940,19 @@
             <v>90</v>
           </cell>
           <cell r="D9">
-            <v>0.74143205177162796</v>
+            <v>339.1</v>
           </cell>
           <cell r="E9">
-            <v>339.11418097653302</v>
+            <v>0.74099999999999999</v>
+          </cell>
+          <cell r="F9">
+            <v>0.82</v>
+          </cell>
+          <cell r="G9">
+            <v>2.2400000000000002</v>
+          </cell>
+          <cell r="H9">
+            <v>4.03</v>
           </cell>
         </row>
         <row r="10">
@@ -819,10 +963,19 @@
             <v>50</v>
           </cell>
           <cell r="D10">
-            <v>0.87493746232692504</v>
+            <v>143.6</v>
           </cell>
           <cell r="E10">
-            <v>143.57829228489899</v>
+            <v>0.875</v>
+          </cell>
+          <cell r="F10">
+            <v>0.26</v>
+          </cell>
+          <cell r="G10">
+            <v>2.4300000000000002</v>
+          </cell>
+          <cell r="H10">
+            <v>6.6</v>
           </cell>
         </row>
         <row r="11">
@@ -833,10 +986,61 @@
             <v>50</v>
           </cell>
           <cell r="D11">
-            <v>0.85825277441075398</v>
+            <v>149.80000000000001</v>
           </cell>
           <cell r="E11">
-            <v>149.83986509868799</v>
+            <v>0.85799999999999998</v>
+          </cell>
+          <cell r="F11">
+            <v>0.28000000000000003</v>
+          </cell>
+          <cell r="G11">
+            <v>2.06</v>
+          </cell>
+          <cell r="H11">
+            <v>5.29</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>c6s</v>
+          </cell>
+          <cell r="F12">
+            <v>1.07</v>
+          </cell>
+          <cell r="G12">
+            <v>5.01</v>
+          </cell>
+          <cell r="H12">
+            <v>10.24</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>c4s</v>
+          </cell>
+          <cell r="F13">
+            <v>2.02</v>
+          </cell>
+          <cell r="G13">
+            <v>9.67</v>
+          </cell>
+          <cell r="H13">
+            <v>15.49</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>c3s</v>
+          </cell>
+          <cell r="F14">
+            <v>0.73</v>
+          </cell>
+          <cell r="G14">
+            <v>2.3199999999999998</v>
+          </cell>
+          <cell r="H14">
+            <v>4.18</v>
           </cell>
         </row>
       </sheetData>
@@ -1162,24 +1366,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="4" width="22.5546875" customWidth="1"/>
     <col min="5" max="5" width="68.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="10" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.33203125" customWidth="1"/>
     <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -1192,29 +1397,29 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="K1">
+      <c r="L1" s="12">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="M1" s="12">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1230,24 +1435,36 @@
       <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" s="1" t="str">
         <f>[1]acc_table!B2</f>
         <v>isim2.con</v>
       </c>
-      <c r="G2">
+      <c r="H2" s="1">
         <f>[1]acc_table!C2</f>
         <v>56</v>
       </c>
-      <c r="H2">
+      <c r="I2" s="1">
         <f>[1]acc_table!D2</f>
-        <v>0.774896281836155</v>
-      </c>
-      <c r="I2">
+        <v>199.8</v>
+      </c>
+      <c r="J2" s="1">
         <f>[1]acc_table!E2</f>
-        <v>199.798864765536</v>
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="K2" s="1">
+        <f>[1]acc_table!F2</f>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="L2" s="1">
+        <f>[1]acc_table!G2</f>
+        <v>2.34</v>
+      </c>
+      <c r="M2" s="1">
+        <f>[1]acc_table!H2</f>
+        <v>5.26</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1263,24 +1480,36 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" s="3" t="str">
         <f>[1]acc_table!B3</f>
         <v>ISI2.agg</v>
       </c>
-      <c r="G3">
+      <c r="H3" s="3">
         <f>[1]acc_table!C3</f>
         <v>90</v>
       </c>
-      <c r="H3">
+      <c r="I3" s="3">
         <f>[1]acc_table!D3</f>
-        <v>0.695859490464528</v>
-      </c>
-      <c r="I3">
+        <v>351.7</v>
+      </c>
+      <c r="J3" s="3">
         <f>[1]acc_table!E3</f>
-        <v>351.72399634026101</v>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="K3" s="3">
+        <f>[1]acc_table!F3</f>
+        <v>0.4</v>
+      </c>
+      <c r="L3" s="3">
+        <f>[1]acc_table!G3</f>
+        <v>1.6</v>
+      </c>
+      <c r="M3" s="3">
+        <f>[1]acc_table!H3</f>
+        <v>3.59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1296,24 +1525,39 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="str">
+      <c r="G4" s="3" t="str">
         <f>[1]acc_table!B4</f>
         <v>ISI2SFC.agg</v>
       </c>
-      <c r="G4">
+      <c r="H4" s="3">
         <f>[1]acc_table!C4</f>
         <v>82</v>
       </c>
-      <c r="H4">
+      <c r="I4" s="3">
         <f>[1]acc_table!D4</f>
-        <v>0.75620344033680598</v>
-      </c>
-      <c r="I4">
+        <v>306.2</v>
+      </c>
+      <c r="J4" s="3">
         <f>[1]acc_table!E4</f>
-        <v>306.18379831355401</v>
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="K4" s="3">
+        <f>[1]acc_table!F4</f>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L4" s="3">
+        <f>[1]acc_table!G4</f>
+        <v>2.21</v>
+      </c>
+      <c r="M4" s="3">
+        <f>[1]acc_table!H4</f>
+        <v>3.97</v>
+      </c>
+      <c r="N4" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1329,24 +1573,36 @@
       <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="str">
+      <c r="G5" s="3" t="str">
         <f>[1]acc_table!B5</f>
         <v>isim2.agg</v>
       </c>
-      <c r="G5">
+      <c r="H5" s="3">
         <f>[1]acc_table!C5</f>
         <v>90</v>
       </c>
-      <c r="H5">
+      <c r="I5" s="3">
         <f>[1]acc_table!D5</f>
-        <v>0.76312115633353605</v>
-      </c>
-      <c r="I5">
+        <v>329.2</v>
+      </c>
+      <c r="J5" s="3">
         <f>[1]acc_table!E5</f>
-        <v>329.22930681027799</v>
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="K5" s="3">
+        <f>[1]acc_table!F5</f>
+        <v>0.42</v>
+      </c>
+      <c r="L5" s="3">
+        <f>[1]acc_table!G5</f>
+        <v>1.67</v>
+      </c>
+      <c r="M5" s="3">
+        <f>[1]acc_table!H5</f>
+        <v>3.76</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1362,24 +1618,39 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6" s="3" t="str">
         <f>[1]acc_table!B6</f>
         <v>isim2SFC.agg</v>
       </c>
-      <c r="G6">
+      <c r="H6" s="3">
         <f>[1]acc_table!C6</f>
         <v>82</v>
       </c>
-      <c r="H6">
+      <c r="I6" s="3">
         <f>[1]acc_table!D6</f>
-        <v>0.80728637787344004</v>
-      </c>
-      <c r="I6">
+        <v>286.89999999999998</v>
+      </c>
+      <c r="J6" s="3">
         <f>[1]acc_table!E6</f>
-        <v>286.90323328026898</v>
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="K6" s="3">
+        <f>[1]acc_table!F6</f>
+        <v>0.9</v>
+      </c>
+      <c r="L6" s="3">
+        <f>[1]acc_table!G6</f>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="M6" s="3">
+        <f>[1]acc_table!H6</f>
+        <v>3.97</v>
+      </c>
+      <c r="N6" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1395,24 +1666,36 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7" s="3" t="str">
         <f>[1]acc_table!B7</f>
         <v>crisi.agg</v>
       </c>
-      <c r="G7">
+      <c r="H7" s="3">
         <f>[1]acc_table!C7</f>
         <v>90</v>
       </c>
-      <c r="H7">
+      <c r="I7" s="3">
         <f>[1]acc_table!D7</f>
-        <v>0.74207775828477995</v>
-      </c>
-      <c r="I7">
+        <v>338.9</v>
+      </c>
+      <c r="J7" s="3">
         <f>[1]acc_table!E7</f>
-        <v>338.88914817787901</v>
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="K7" s="3">
+        <f>[1]acc_table!F7</f>
+        <v>0.68</v>
+      </c>
+      <c r="L7" s="3">
+        <f>[1]acc_table!G7</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="M7" s="3">
+        <f>[1]acc_table!H7</f>
+        <v>4.22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1428,24 +1711,36 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8" s="3" t="str">
         <f>[1]acc_table!B8</f>
         <v>crisim.agg</v>
       </c>
-      <c r="G8">
+      <c r="H8" s="3">
         <f>[1]acc_table!C8</f>
         <v>90</v>
       </c>
-      <c r="H8">
+      <c r="I8" s="3">
         <f>[1]acc_table!D8</f>
-        <v>0.77352340243057605</v>
-      </c>
-      <c r="I8">
+        <v>327.2</v>
+      </c>
+      <c r="J8" s="3">
         <f>[1]acc_table!E8</f>
-        <v>327.18766019001299</v>
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="K8" s="3">
+        <f>[1]acc_table!F8</f>
+        <v>0.65</v>
+      </c>
+      <c r="L8" s="3">
+        <f>[1]acc_table!G8</f>
+        <v>2.17</v>
+      </c>
+      <c r="M8" s="3">
+        <f>[1]acc_table!H8</f>
+        <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1461,24 +1756,36 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9" s="3" t="str">
         <f>[1]acc_table!B9</f>
         <v>axb.isi.agg</v>
       </c>
-      <c r="G9">
+      <c r="H9" s="3">
         <f>[1]acc_table!C9</f>
         <v>90</v>
       </c>
-      <c r="H9">
+      <c r="I9" s="3">
         <f>[1]acc_table!D9</f>
-        <v>0.74143205177162796</v>
-      </c>
-      <c r="I9">
+        <v>339.1</v>
+      </c>
+      <c r="J9" s="3">
         <f>[1]acc_table!E9</f>
-        <v>339.11418097653302</v>
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="K9" s="3">
+        <f>[1]acc_table!F9</f>
+        <v>0.82</v>
+      </c>
+      <c r="L9" s="3">
+        <f>[1]acc_table!G9</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="M9" s="3">
+        <f>[1]acc_table!H9</f>
+        <v>4.03</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1494,24 +1801,36 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" t="str">
+      <c r="G10" s="1" t="str">
         <f>[1]acc_table!B10</f>
         <v>crisi.con</v>
       </c>
-      <c r="G10">
+      <c r="H10" s="7">
         <f>[1]acc_table!C10</f>
         <v>50</v>
       </c>
-      <c r="H10">
+      <c r="I10" s="1">
         <f>[1]acc_table!D10</f>
-        <v>0.87493746232692504</v>
-      </c>
-      <c r="I10">
+        <v>143.6</v>
+      </c>
+      <c r="J10" s="1">
         <f>[1]acc_table!E10</f>
-        <v>143.57829228489899</v>
+        <v>0.875</v>
+      </c>
+      <c r="K10" s="1">
+        <f>[1]acc_table!F10</f>
+        <v>0.26</v>
+      </c>
+      <c r="L10" s="1">
+        <f>[1]acc_table!G10</f>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="M10" s="1">
+        <f>[1]acc_table!H10</f>
+        <v>6.6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1527,42 +1846,231 @@
       <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11" s="2" t="str">
         <f>[1]acc_table!B11</f>
         <v>crisim.con</v>
       </c>
-      <c r="G11">
+      <c r="H11" s="2">
         <f>[1]acc_table!C11</f>
         <v>50</v>
       </c>
-      <c r="H11">
+      <c r="I11" s="2">
         <f>[1]acc_table!D11</f>
-        <v>0.85825277441075398</v>
-      </c>
-      <c r="I11">
+        <v>149.80000000000001</v>
+      </c>
+      <c r="J11" s="2">
         <f>[1]acc_table!E11</f>
-        <v>149.83986509868799</v>
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="K11" s="2">
+        <f>[1]acc_table!F11</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="L11" s="2">
+        <f>[1]acc_table!G11</f>
+        <v>2.06</v>
+      </c>
+      <c r="M11" s="2">
+        <f>[1]acc_table!H11</f>
+        <v>5.29</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G12" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="4">
+        <f>AVERAGE(K3:K9)</f>
+        <v>0.71857142857142864</v>
+      </c>
+      <c r="L12" s="4">
+        <f>AVERAGE(L3:L9)</f>
+        <v>2.0257142857142858</v>
+      </c>
+      <c r="M12" s="4">
+        <f>AVERAGE(M3:M9)</f>
+        <v>3.9542857142857146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G13" s="14">
+        <v>0.35</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="4">
+        <f>K12*1.35</f>
+        <v>0.9700714285714287</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" ref="L13:M13" si="0">L12*1.35</f>
+        <v>2.7347142857142859</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="0"/>
+        <v>5.338285714285715</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G14" s="15">
+        <v>-0.35</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="6">
+        <f>K12*0.65</f>
+        <v>0.46707142857142864</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" ref="L14:M14" si="1">L12*0.65</f>
+        <v>1.3167142857142857</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="1"/>
+        <v>2.5702857142857147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>14</v>
       </c>
+      <c r="G15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8">
+        <f>AVERAGE(K2,K10:K11)</f>
+        <v>0.37333333333333335</v>
+      </c>
+      <c r="L15" s="8">
+        <f>AVERAGE(L2,L10:L11)</f>
+        <v>2.2766666666666668</v>
+      </c>
+      <c r="M15" s="8">
+        <f>AVERAGE(M2,M10:M11)</f>
+        <v>5.7166666666666659</v>
+      </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>16</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
+      <c r="G16" s="17">
+        <v>0.35</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8">
+        <f>K15*1.35</f>
+        <v>0.504</v>
+      </c>
+      <c r="L16" s="8">
+        <f t="shared" ref="L16" si="2">L15*1.35</f>
+        <v>3.0735000000000006</v>
+      </c>
+      <c r="M16" s="8">
+        <f t="shared" ref="M16" si="3">M15*1.35</f>
+        <v>7.7174999999999994</v>
+      </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>16</v>
       </c>
       <c r="E17" t="s">
         <v>22</v>
+      </c>
+      <c r="G17" s="18">
+        <v>-0.35</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="10">
+        <f>K15*0.65</f>
+        <v>0.2426666666666667</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" ref="L17:M17" si="4">L15*0.65</f>
+        <v>1.4798333333333336</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="4"/>
+        <v>3.7158333333333329</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G18" s="11" t="str">
+        <f>[1]acc_table!B12</f>
+        <v>c6s</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11">
+        <f>[1]acc_table!F12</f>
+        <v>1.07</v>
+      </c>
+      <c r="L18" s="11">
+        <f>[1]acc_table!G12</f>
+        <v>5.01</v>
+      </c>
+      <c r="M18" s="11">
+        <f>[1]acc_table!H12</f>
+        <v>10.24</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G19" s="11" t="str">
+        <f>[1]acc_table!B13</f>
+        <v>c4s</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11">
+        <f>[1]acc_table!F13</f>
+        <v>2.02</v>
+      </c>
+      <c r="L19" s="11">
+        <f>[1]acc_table!G13</f>
+        <v>9.67</v>
+      </c>
+      <c r="M19" s="11">
+        <f>[1]acc_table!H13</f>
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="G20" s="11" t="str">
+        <f>[1]acc_table!B14</f>
+        <v>c3s</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11">
+        <f>[1]acc_table!F14</f>
+        <v>0.73</v>
+      </c>
+      <c r="L20" s="11">
+        <f>[1]acc_table!G14</f>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="M20" s="11">
+        <f>[1]acc_table!H14</f>
+        <v>4.18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Starting to work on Discussion
</commit_message>
<xml_diff>
--- a/acc_table.xlsx
+++ b/acc_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dan\_Remote_projects\ccp-sROS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D38B70-94A4-4940-833B-0753EC3EFDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCEFCBE-675D-4BDE-867F-8534E64D598C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>Model</t>
   </si>
@@ -138,38 +138,76 @@
     <t>c6s</t>
   </si>
   <si>
-    <t>C6s</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
     <t>c4s</t>
   </si>
   <si>
-    <t>C4s</t>
-  </si>
-  <si>
     <t>c3s</t>
   </si>
   <si>
-    <t>C3s</t>
-  </si>
-  <si>
     <t>d1</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>Step 1: copy acc_table.csv to 'csv copy' worksheet</t>
+    <t>~ 30 * (1-exp(-0.08*ISI))^3</t>
+  </si>
+  <si>
+    <t>~ 20 * (1-exp(-0.2*ISI))^5</t>
+  </si>
+  <si>
+    <t>~ 15 * (1-exp(-0.05*ISI))^2</t>
+  </si>
+  <si>
+    <t>~ 30 * (1-exp(-0.0232*ISI))^1.6</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <r>
+      <t>E R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Models using ISI are unshaded, those using ISIsa are lightly shaded and FBP-era surface model  predictions are shown (dark shading) for comparison (see text for details).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table 1. Summary of predictors, number of observations (n), model predictions at three levels of ISI / ISIsa and evalution measures for fitted models. </t>
+  </si>
+  <si>
+    <t>Predicted ROS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBP-era surface ROS model formulae are as per Forestry Canada Fire Danger Group 1992 (C6s, D1) and Van Wagner 1993 (C4s, C3s; see text). </t>
+  </si>
+  <si>
+    <t>[Step 1: copy acc_table.csv to 'csv copy' worksheet]</t>
+  </si>
+  <si>
+    <t>For Model 3, ISI predictions assume FFMC of 91. For Models 5 and 7 requiring estimated SFC, predictions were calculated at SFC=1.5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RMSE is root mean squared error, MAE is mean absolute error, MAPE is mean absolute percentage error, E R2 is Efron's R-squared, and AIC is Akaike's Information Criterion. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,6 +338,15 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -675,9 +722,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -688,6 +732,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1074,877 +1121,912 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="5" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" customWidth="1"/>
+    <col min="5" max="7" width="5.77734375" customWidth="1"/>
+    <col min="8" max="11" width="6.109375" customWidth="1"/>
+    <col min="12" max="12" width="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="str">
+      <c r="E1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="str">
+        <f>'CSV copy'!C1</f>
+        <v>Num</v>
+      </c>
+      <c r="B2" s="1" t="str">
         <f>'CSV copy'!D1</f>
         <v>Model</v>
       </c>
-      <c r="C1" s="2" t="str">
+      <c r="C2" s="1" t="str">
         <f>'CSV copy'!E1</f>
         <v>Formula</v>
       </c>
-      <c r="D1" s="2" t="str">
-        <f>'CSV copy'!F1</f>
-        <v>nobs</v>
-      </c>
-      <c r="E1" s="2" t="str">
+      <c r="D2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="1" t="str">
         <f>'CSV copy'!G1</f>
         <v>ISI.5</v>
       </c>
-      <c r="F1" s="2" t="str">
+      <c r="F2" s="1" t="str">
         <f>'CSV copy'!H1</f>
         <v>ISI.10</v>
       </c>
-      <c r="G1" s="2" t="str">
+      <c r="G2" s="1" t="str">
         <f>'CSV copy'!I1</f>
         <v>ISI.15</v>
       </c>
-      <c r="H1" s="2" t="str">
+      <c r="H2" s="1" t="str">
         <f>'CSV copy'!J1</f>
         <v>RMSE</v>
       </c>
-      <c r="I1" s="2" t="str">
+      <c r="I2" s="1" t="str">
         <f>'CSV copy'!K1</f>
         <v>MAE</v>
       </c>
-      <c r="J1" s="2" t="str">
+      <c r="J2" s="1" t="str">
         <f>'CSV copy'!L1</f>
         <v>MAPE</v>
       </c>
-      <c r="K1" s="2" t="str">
-        <f>'CSV copy'!M1</f>
-        <v>EfronR2</v>
-      </c>
-      <c r="L1" s="2" t="str">
+      <c r="K2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="1" t="str">
         <f>'CSV copy'!N1</f>
         <v>AIC</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <f>'CSV copy'!C2</f>
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="str">
+      <c r="B3" s="3" t="str">
         <f>'CSV copy'!D2</f>
         <v>isi.lin</v>
       </c>
-      <c r="C2" s="4" t="str">
+      <c r="C3" s="3" t="str">
         <f>'CSV copy'!E2</f>
         <v>~ ISI</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D3" s="3">
         <f>'CSV copy'!F2</f>
         <v>56</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E3" s="3">
         <f>'CSV copy'!G2</f>
         <v>0.66</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F3" s="3">
         <f>'CSV copy'!H2</f>
         <v>3.09</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G3" s="3">
         <f>'CSV copy'!I2</f>
         <v>5.51</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H3" s="3">
         <f>'CSV copy'!J2</f>
         <v>1.53</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I3" s="3">
         <f>'CSV copy'!K2</f>
         <v>1.1399999999999999</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J3" s="3">
         <f>'CSV copy'!L2</f>
         <v>0.85099999999999998</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K3" s="3">
         <f>'CSV copy'!M2</f>
         <v>0.46899999999999997</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L3" s="3">
         <f>'CSV copy'!N2</f>
         <v>212.3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <f>'CSV copy'!C3</f>
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="str">
+      <c r="B4" s="2" t="str">
         <f>'CSV copy'!D3</f>
         <v>isim2.con</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C4" s="2" t="str">
         <f>'CSV copy'!E3</f>
         <v>~ I(isi.m^2) - 1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D4" s="2">
         <f>'CSV copy'!F3</f>
         <v>56</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E4" s="2">
         <f>'CSV copy'!G3</f>
         <v>0.57999999999999996</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F4" s="2">
         <f>'CSV copy'!H3</f>
         <v>2.34</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G4" s="2">
         <f>'CSV copy'!I3</f>
         <v>5.26</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H4" s="2">
         <f>'CSV copy'!J3</f>
         <v>1.39</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I4" s="2">
         <f>'CSV copy'!K3</f>
         <v>0.98399999999999999</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J4" s="2">
         <f>'CSV copy'!L3</f>
         <v>0.63900000000000001</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K4" s="2">
         <f>'CSV copy'!M3</f>
         <v>0.56000000000000005</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L4" s="2">
         <f>'CSV copy'!N3</f>
         <v>199.8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <f>'CSV copy'!C4</f>
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="str">
+      <c r="B5" s="3" t="str">
         <f>'CSV copy'!D4</f>
         <v>WS2.agg</v>
       </c>
-      <c r="C4" s="4" t="str">
+      <c r="C5" s="3" t="str">
         <f>'CSV copy'!E4</f>
         <v>~ I(ws^2) - 1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D5" s="3">
         <f>'CSV copy'!F4</f>
         <v>91</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E5" s="3">
         <f>'CSV copy'!G4</f>
         <v>0.01</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F5" s="3">
         <f>'CSV copy'!H4</f>
         <v>1.98</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G5" s="3">
         <f>'CSV copy'!I4</f>
         <v>4.88</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H5" s="3">
         <f>'CSV copy'!J4</f>
         <v>1.92</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I5" s="3">
         <f>'CSV copy'!K4</f>
         <v>1.25</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J5" s="3">
         <f>'CSV copy'!L4</f>
         <v>0.65900000000000003</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K5" s="3">
         <f>'CSV copy'!M4</f>
         <v>0.26</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L5" s="3">
         <f>'CSV copy'!N4</f>
         <v>380.9</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <f>'CSV copy'!C5</f>
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="str">
+      <c r="B6" s="3" t="str">
         <f>'CSV copy'!D5</f>
         <v>ISI2.agg</v>
       </c>
-      <c r="C5" s="4" t="str">
+      <c r="C6" s="3" t="str">
         <f>'CSV copy'!E5</f>
         <v>~ I(ISI^2) - 1</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="3">
         <f>'CSV copy'!F5</f>
         <v>91</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E6" s="3">
         <f>'CSV copy'!G5</f>
         <v>0.41</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F6" s="3">
         <f>'CSV copy'!H5</f>
         <v>1.64</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G6" s="3">
         <f>'CSV copy'!I5</f>
         <v>3.7</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H6" s="3">
         <f>'CSV copy'!J5</f>
         <v>1.78</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I6" s="3">
         <f>'CSV copy'!K5</f>
         <v>1.19</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J6" s="3">
         <f>'CSV copy'!L5</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K6" s="3">
         <f>'CSV copy'!M5</f>
         <v>0.36399999999999999</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L6" s="3">
         <f>'CSV copy'!N5</f>
         <v>367.2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <f>'CSV copy'!C6</f>
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="str">
+      <c r="B7" s="3" t="str">
         <f>'CSV copy'!D6</f>
         <v>ISI2SFC.agg</v>
       </c>
-      <c r="C6" s="4" t="str">
+      <c r="C7" s="3" t="str">
         <f>'CSV copy'!E6</f>
         <v>~ I(ISI^2) + sqrt(SFC) - 1</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D7" s="3">
         <f>'CSV copy'!F6</f>
         <v>84</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E7" s="3">
         <f>'CSV copy'!G6</f>
         <v>1.49</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F7" s="3">
         <f>'CSV copy'!H6</f>
         <v>2.48</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G7" s="3">
         <f>'CSV copy'!I6</f>
         <v>4.13</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H7" s="3">
         <f>'CSV copy'!J6</f>
         <v>1.58</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I7" s="3">
         <f>'CSV copy'!K6</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J7" s="3">
         <f>'CSV copy'!L6</f>
         <v>0.73</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K7" s="3">
         <f>'CSV copy'!M6</f>
         <v>0.51800000000000002</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L7" s="3">
         <f>'CSV copy'!N6</f>
         <v>320.8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <f>'CSV copy'!C7</f>
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="str">
+      <c r="B8" s="2" t="str">
         <f>'CSV copy'!D7</f>
         <v>isim2.agg</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C8" s="2" t="str">
         <f>'CSV copy'!E7</f>
         <v>~ I(isi.m^2) - 1</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="2">
         <f>'CSV copy'!F7</f>
         <v>91</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E8" s="2">
         <f>'CSV copy'!G7</f>
         <v>0.44</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F8" s="2">
         <f>'CSV copy'!H7</f>
         <v>1.76</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G8" s="2">
         <f>'CSV copy'!I7</f>
         <v>3.96</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H8" s="2">
         <f>'CSV copy'!J7</f>
         <v>1.47</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I8" s="2">
         <f>'CSV copy'!K7</f>
         <v>1.05</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J8" s="2">
         <f>'CSV copy'!L7</f>
         <v>0.56200000000000006</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K8" s="2">
         <f>'CSV copy'!M7</f>
         <v>0.56699999999999995</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L8" s="2">
         <f>'CSV copy'!N7</f>
         <v>332.2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <f>'CSV copy'!C8</f>
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="str">
+      <c r="B9" s="2" t="str">
         <f>'CSV copy'!D8</f>
         <v>isim2SFC.agg</v>
       </c>
-      <c r="C8" s="3" t="str">
+      <c r="C9" s="2" t="str">
         <f>'CSV copy'!E8</f>
         <v>~ I(isi.m^2) + sqrt(SFC) - 1</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="2">
         <f>'CSV copy'!F8</f>
         <v>84</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E9" s="2">
         <f>'CSV copy'!G8</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F9" s="2">
         <f>'CSV copy'!H8</f>
         <v>2.2599999999999998</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G9" s="2">
         <f>'CSV copy'!I8</f>
         <v>4.18</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H9" s="2">
         <f>'CSV copy'!J8</f>
         <v>1.31</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I9" s="2">
         <f>'CSV copy'!K8</f>
         <v>0.95299999999999996</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J9" s="2">
         <f>'CSV copy'!L8</f>
         <v>0.59899999999999998</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K9" s="2">
         <f>'CSV copy'!M8</f>
         <v>0.66400000000000003</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L9" s="2">
         <f>'CSV copy'!N8</f>
         <v>290.3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <f>'CSV copy'!C9</f>
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="str">
+      <c r="B10" s="3" t="str">
         <f>'CSV copy'!D9</f>
         <v>crisi.agg</v>
       </c>
-      <c r="C9" s="4" t="str">
+      <c r="C10" s="3" t="str">
         <f>'CSV copy'!E9</f>
         <v>~ 25 * (1 - exp(-b * ISI))^c</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D10" s="3">
         <f>'CSV copy'!F9</f>
         <v>91</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E10" s="3">
         <f>'CSV copy'!G9</f>
         <v>0.77</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F10" s="3">
         <f>'CSV copy'!H9</f>
         <v>2.38</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G10" s="3">
         <f>'CSV copy'!I9</f>
         <v>4.3600000000000003</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H10" s="3">
         <f>'CSV copy'!J9</f>
         <v>1.62</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I10" s="3">
         <f>'CSV copy'!K9</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J10" s="3">
         <f>'CSV copy'!L9</f>
         <v>0.73399999999999999</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K10" s="3">
         <f>'CSV copy'!M9</f>
         <v>0.47599999999999998</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L10" s="3">
         <f>'CSV copy'!N9</f>
         <v>351.5</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <f>'CSV copy'!C10</f>
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="str">
+      <c r="B11" s="2" t="str">
         <f>'CSV copy'!D10</f>
         <v>crisim.agg</v>
       </c>
-      <c r="C10" s="3" t="str">
+      <c r="C11" s="2" t="str">
         <f>'CSV copy'!E10</f>
         <v>~ 25 * (1 - exp(-b * isi.m))^c</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="2">
         <f>'CSV copy'!F10</f>
         <v>91</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E11" s="2">
         <f>'CSV copy'!G10</f>
         <v>0.65</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F11" s="2">
         <f>'CSV copy'!H10</f>
         <v>2.27</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G11" s="2">
         <f>'CSV copy'!I10</f>
         <v>4.38</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H11" s="2">
         <f>'CSV copy'!J10</f>
         <v>1.42</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I11" s="2">
         <f>'CSV copy'!K10</f>
         <v>1.04</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J11" s="2">
         <f>'CSV copy'!L10</f>
         <v>0.65300000000000002</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K11" s="2">
         <f>'CSV copy'!M10</f>
         <v>0.59499999999999997</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L11" s="2">
         <f>'CSV copy'!N10</f>
         <v>328.1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <f>'CSV copy'!C11</f>
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="str">
+      <c r="B12" s="3" t="str">
         <f>'CSV copy'!D11</f>
         <v>axb.isi.agg</v>
       </c>
-      <c r="C11" s="4" t="str">
+      <c r="C12" s="3" t="str">
         <f>'CSV copy'!E11</f>
         <v>~ a * ISI^b</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D12" s="3">
         <f>'CSV copy'!F11</f>
         <v>91</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E12" s="3">
         <f>'CSV copy'!G11</f>
         <v>0.9</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F12" s="3">
         <f>'CSV copy'!H11</f>
         <v>2.37</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G12" s="3">
         <f>'CSV copy'!I11</f>
         <v>4.17</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H12" s="3">
         <f>'CSV copy'!J11</f>
         <v>1.62</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I12" s="3">
         <f>'CSV copy'!K11</f>
         <v>1.17</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J12" s="3">
         <f>'CSV copy'!L11</f>
         <v>0.749</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K12" s="3">
         <f>'CSV copy'!M11</f>
         <v>0.47399999999999998</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L12" s="3">
         <f>'CSV copy'!N11</f>
         <v>352</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <f>'CSV copy'!C12</f>
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="str">
+      <c r="B13" s="3" t="str">
         <f>'CSV copy'!D12</f>
         <v>crisi.con</v>
       </c>
-      <c r="C12" s="4" t="str">
+      <c r="C13" s="3" t="str">
         <f>'CSV copy'!E12</f>
         <v>~ 25 * (1 - exp(-b * ISI))^c</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D13" s="3">
         <f>'CSV copy'!F12</f>
         <v>51</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E13" s="3">
         <f>'CSV copy'!G12</f>
         <v>0.27</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F13" s="3">
         <f>'CSV copy'!H12</f>
         <v>2.5099999999999998</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="3">
         <f>'CSV copy'!I12</f>
         <v>6.76</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H13" s="3">
         <f>'CSV copy'!J12</f>
         <v>0.98</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I13" s="3">
         <f>'CSV copy'!K12</f>
         <v>0.77900000000000003</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J13" s="3">
         <f>'CSV copy'!L12</f>
         <v>0.59899999999999998</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K13" s="3">
         <f>'CSV copy'!M12</f>
         <v>0.78100000000000003</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L13" s="3">
         <f>'CSV copy'!N12</f>
         <v>148.69999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <f>'CSV copy'!C13</f>
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="str">
+      <c r="B14" s="2" t="str">
         <f>'CSV copy'!D13</f>
         <v>crisim.con</v>
       </c>
-      <c r="C13" s="3" t="str">
+      <c r="C14" s="2" t="str">
         <f>'CSV copy'!E13</f>
         <v>~ 25 * (1 - exp(-b * isi.m))^c</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D14" s="2">
         <f>'CSV copy'!F13</f>
         <v>51</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="2">
         <f>'CSV copy'!G13</f>
         <v>0.32</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F14" s="2">
         <f>'CSV copy'!H13</f>
         <v>2.1800000000000002</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G14" s="2">
         <f>'CSV copy'!I13</f>
         <v>5.45</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H14" s="2">
         <f>'CSV copy'!J13</f>
         <v>1.08</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I14" s="2">
         <f>'CSV copy'!K13</f>
         <v>0.85199999999999998</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J14" s="2">
         <f>'CSV copy'!L13</f>
         <v>0.64600000000000002</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K14" s="2">
         <f>'CSV copy'!M13</f>
         <v>0.73299999999999998</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L14" s="2">
         <f>'CSV copy'!N13</f>
         <v>158.80000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
         <f>'CSV copy'!C14</f>
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="str">
+      <c r="B15" s="4" t="str">
         <f>'CSV copy'!D14</f>
         <v>c6s</v>
       </c>
-      <c r="C14" s="5" t="str">
+      <c r="C15" s="4" t="str">
         <f>'CSV copy'!E14</f>
-        <v>C6s</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f>'CSV copy'!F14</f>
-        <v>NA</v>
-      </c>
-      <c r="E14" s="5">
+        <v>~ 30 * (1-exp(-0.08*ISI))^3</v>
+      </c>
+      <c r="D15" s="4" t="str">
+        <f>IF('CSV copy'!F14="NA", "-", 'CSV copy'!F14)</f>
+        <v>-</v>
+      </c>
+      <c r="E15" s="4">
         <f>'CSV copy'!G14</f>
         <v>1.07</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F15" s="4">
         <f>'CSV copy'!H14</f>
         <v>5.01</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G15" s="4">
         <f>'CSV copy'!I14</f>
         <v>10.24</v>
       </c>
-      <c r="H14" s="4" t="str">
-        <f>'CSV copy'!J14</f>
-        <v>NA</v>
-      </c>
-      <c r="I14" s="4" t="str">
-        <f>'CSV copy'!K14</f>
-        <v>NA</v>
-      </c>
-      <c r="J14" s="4" t="str">
-        <f>'CSV copy'!L14</f>
-        <v>NA</v>
-      </c>
-      <c r="K14" s="4" t="str">
-        <f>'CSV copy'!M14</f>
-        <v>NA</v>
-      </c>
-      <c r="L14" s="4" t="str">
-        <f>'CSV copy'!N14</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+      <c r="H15" s="3" t="str">
+        <f>IF('CSV copy'!J14="NA", "-", 'CSV copy'!J14)</f>
+        <v>-</v>
+      </c>
+      <c r="I15" s="3" t="str">
+        <f>IF('CSV copy'!K14="NA", "-", 'CSV copy'!K14)</f>
+        <v>-</v>
+      </c>
+      <c r="J15" s="3" t="str">
+        <f>IF('CSV copy'!L14="NA", "-", 'CSV copy'!L14)</f>
+        <v>-</v>
+      </c>
+      <c r="K15" s="3" t="str">
+        <f>IF('CSV copy'!M14="NA", "-", 'CSV copy'!M14)</f>
+        <v>-</v>
+      </c>
+      <c r="L15" s="3" t="str">
+        <f>IF('CSV copy'!N14="NA", "-", 'CSV copy'!N14)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
         <f>'CSV copy'!C15</f>
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="str">
+      <c r="B16" s="4" t="str">
         <f>'CSV copy'!D15</f>
         <v>c4s</v>
       </c>
-      <c r="C15" s="5" t="str">
+      <c r="C16" s="4" t="str">
         <f>'CSV copy'!E15</f>
-        <v>C4s</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <f>'CSV copy'!F15</f>
-        <v>NA</v>
-      </c>
-      <c r="E15" s="5">
+        <v>~ 20 * (1-exp(-0.2*ISI))^5</v>
+      </c>
+      <c r="D16" s="4" t="str">
+        <f>IF('CSV copy'!F15="NA", "-", 'CSV copy'!F15)</f>
+        <v>-</v>
+      </c>
+      <c r="E16" s="4">
         <f>'CSV copy'!G15</f>
         <v>2.02</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F16" s="4">
         <f>'CSV copy'!H15</f>
         <v>9.67</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G16" s="4">
         <f>'CSV copy'!I15</f>
         <v>15.49</v>
       </c>
-      <c r="H15" s="4" t="str">
-        <f>'CSV copy'!J15</f>
-        <v>NA</v>
-      </c>
-      <c r="I15" s="4" t="str">
-        <f>'CSV copy'!K15</f>
-        <v>NA</v>
-      </c>
-      <c r="J15" s="4" t="str">
-        <f>'CSV copy'!L15</f>
-        <v>NA</v>
-      </c>
-      <c r="K15" s="4" t="str">
-        <f>'CSV copy'!M15</f>
-        <v>NA</v>
-      </c>
-      <c r="L15" s="4" t="str">
-        <f>'CSV copy'!N15</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+      <c r="H16" s="3" t="str">
+        <f>IF('CSV copy'!J15="NA", "-", 'CSV copy'!J15)</f>
+        <v>-</v>
+      </c>
+      <c r="I16" s="3" t="str">
+        <f>IF('CSV copy'!K15="NA", "-", 'CSV copy'!K15)</f>
+        <v>-</v>
+      </c>
+      <c r="J16" s="3" t="str">
+        <f>IF('CSV copy'!L15="NA", "-", 'CSV copy'!L15)</f>
+        <v>-</v>
+      </c>
+      <c r="K16" s="3" t="str">
+        <f>IF('CSV copy'!M15="NA", "-", 'CSV copy'!M15)</f>
+        <v>-</v>
+      </c>
+      <c r="L16" s="3" t="str">
+        <f>IF('CSV copy'!N15="NA", "-", 'CSV copy'!N15)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
         <f>'CSV copy'!C16</f>
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="str">
+      <c r="B17" s="4" t="str">
         <f>'CSV copy'!D16</f>
         <v>c3s</v>
       </c>
-      <c r="C16" s="5" t="str">
+      <c r="C17" s="4" t="str">
         <f>'CSV copy'!E16</f>
-        <v>C3s</v>
-      </c>
-      <c r="D16" s="5" t="str">
-        <f>'CSV copy'!F16</f>
-        <v>NA</v>
-      </c>
-      <c r="E16" s="5">
+        <v>~ 15 * (1-exp(-0.05*ISI))^2</v>
+      </c>
+      <c r="D17" s="4" t="str">
+        <f>IF('CSV copy'!F16="NA", "-", 'CSV copy'!F16)</f>
+        <v>-</v>
+      </c>
+      <c r="E17" s="4">
         <f>'CSV copy'!G16</f>
         <v>0.73</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F17" s="4">
         <f>'CSV copy'!H16</f>
         <v>2.3199999999999998</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G17" s="4">
         <f>'CSV copy'!I16</f>
         <v>4.18</v>
       </c>
-      <c r="H16" s="4" t="str">
-        <f>'CSV copy'!J16</f>
-        <v>NA</v>
-      </c>
-      <c r="I16" s="4" t="str">
-        <f>'CSV copy'!K16</f>
-        <v>NA</v>
-      </c>
-      <c r="J16" s="4" t="str">
-        <f>'CSV copy'!L16</f>
-        <v>NA</v>
-      </c>
-      <c r="K16" s="4" t="str">
-        <f>'CSV copy'!M16</f>
-        <v>NA</v>
-      </c>
-      <c r="L16" s="4" t="str">
-        <f>'CSV copy'!N16</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="H17" s="3" t="str">
+        <f>IF('CSV copy'!J16="NA", "-", 'CSV copy'!J16)</f>
+        <v>-</v>
+      </c>
+      <c r="I17" s="3" t="str">
+        <f>IF('CSV copy'!K16="NA", "-", 'CSV copy'!K16)</f>
+        <v>-</v>
+      </c>
+      <c r="J17" s="3" t="str">
+        <f>IF('CSV copy'!L16="NA", "-", 'CSV copy'!L16)</f>
+        <v>-</v>
+      </c>
+      <c r="K17" s="3" t="str">
+        <f>IF('CSV copy'!M16="NA", "-", 'CSV copy'!M16)</f>
+        <v>-</v>
+      </c>
+      <c r="L17" s="3" t="str">
+        <f>IF('CSV copy'!N16="NA", "-", 'CSV copy'!N16)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
         <f>'CSV copy'!C17</f>
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="str">
+      <c r="B18" s="4" t="str">
         <f>'CSV copy'!D17</f>
         <v>d1</v>
       </c>
-      <c r="C17" s="5" t="str">
+      <c r="C18" s="4" t="str">
         <f>'CSV copy'!E17</f>
-        <v>D1</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <f>'CSV copy'!F17</f>
-        <v>NA</v>
-      </c>
-      <c r="E17" s="5">
+        <v>~ 30 * (1-exp(-0.0232*ISI))^1.6</v>
+      </c>
+      <c r="D18" s="4" t="str">
+        <f>IF('CSV copy'!F17="NA", "-", 'CSV copy'!F17)</f>
+        <v>-</v>
+      </c>
+      <c r="E18" s="4">
         <f>'CSV copy'!G17</f>
         <v>0.87</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F18" s="4">
         <f>'CSV copy'!H17</f>
         <v>2.41</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G18" s="4">
         <f>'CSV copy'!I17</f>
         <v>4.2300000000000004</v>
       </c>
-      <c r="H17" s="4" t="str">
-        <f>'CSV copy'!J17</f>
-        <v>NA</v>
-      </c>
-      <c r="I17" s="4" t="str">
-        <f>'CSV copy'!K17</f>
-        <v>NA</v>
-      </c>
-      <c r="J17" s="4" t="str">
-        <f>'CSV copy'!L17</f>
-        <v>NA</v>
-      </c>
-      <c r="K17" s="4" t="str">
-        <f>'CSV copy'!M17</f>
-        <v>NA</v>
-      </c>
-      <c r="L17" s="4" t="str">
-        <f>'CSV copy'!N17</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>42</v>
+      <c r="H18" s="3" t="str">
+        <f>IF('CSV copy'!J17="NA", "-", 'CSV copy'!J17)</f>
+        <v>-</v>
+      </c>
+      <c r="I18" s="3" t="str">
+        <f>IF('CSV copy'!K17="NA", "-", 'CSV copy'!K17)</f>
+        <v>-</v>
+      </c>
+      <c r="J18" s="3" t="str">
+        <f>IF('CSV copy'!L17="NA", "-", 'CSV copy'!L17)</f>
+        <v>-</v>
+      </c>
+      <c r="K18" s="3" t="str">
+        <f>IF('CSV copy'!M17="NA", "-", 'CSV copy'!M17)</f>
+        <v>-</v>
+      </c>
+      <c r="L18" s="3" t="str">
+        <f>IF('CSV copy'!N17="NA", "-", 'CSV copy'!N17)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -1958,7 +2040,7 @@
   <dimension ref="B1:N17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2504,10 +2586,10 @@
         <v>33</v>
       </c>
       <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
-      </c>
-      <c r="F14" t="s">
-        <v>35</v>
       </c>
       <c r="G14">
         <v>1.07</v>
@@ -2519,19 +2601,19 @@
         <v>10.24</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -2542,13 +2624,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G15">
         <v>2.02</v>
@@ -2560,19 +2642,19 @@
         <v>15.49</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -2583,13 +2665,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16">
         <v>0.73</v>
@@ -2601,19 +2683,19 @@
         <v>4.18</v>
       </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
@@ -2624,13 +2706,13 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
         <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17">
         <v>0.87</v>
@@ -2642,19 +2724,19 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>